<commit_message>
Filled the guyz I can
</commit_message>
<xml_diff>
--- a/Timetable/SampleGuide.xlsx
+++ b/Timetable/SampleGuide.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Opsi Jay\Documents\Visual Studio 2017\Projects\Timetable\Timetable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\f\Documents\Visual Studio\TTSS\Timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A45452AD-9E0D-484C-9CA5-F0C7DCEDDA40}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="6960" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="4" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="181">
   <si>
     <t>StudentTable</t>
   </si>
@@ -142,12 +141,441 @@
   </si>
   <si>
     <t>e304</t>
+  </si>
+  <si>
+    <t>Timi</t>
+  </si>
+  <si>
+    <t>Seyi</t>
+  </si>
+  <si>
+    <t>Teni</t>
+  </si>
+  <si>
+    <t>Peace</t>
+  </si>
+  <si>
+    <t>Deji</t>
+  </si>
+  <si>
+    <t>Jedi</t>
+  </si>
+  <si>
+    <t>Chibueze</t>
+  </si>
+  <si>
+    <t>Tola</t>
+  </si>
+  <si>
+    <t>csc405</t>
+  </si>
+  <si>
+    <t>Obinna</t>
+  </si>
+  <si>
+    <t>ssg501</t>
+  </si>
+  <si>
+    <t>ssg502</t>
+  </si>
+  <si>
+    <t>ssg503</t>
+  </si>
+  <si>
+    <t>ssg507</t>
+  </si>
+  <si>
+    <t>ssg 505</t>
+  </si>
+  <si>
+    <t>ssg509</t>
+  </si>
+  <si>
+    <t>Temi</t>
+  </si>
+  <si>
+    <t>ssg504</t>
+  </si>
+  <si>
+    <t>ssg506</t>
+  </si>
+  <si>
+    <t>ssg508</t>
+  </si>
+  <si>
+    <t>ssg510</t>
+  </si>
+  <si>
+    <t>Florian</t>
+  </si>
+  <si>
+    <t>ssg513</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>ssg517</t>
+  </si>
+  <si>
+    <t>ssg514</t>
+  </si>
+  <si>
+    <t>Josh</t>
+  </si>
+  <si>
+    <t>ssg516</t>
+  </si>
+  <si>
+    <t>ssg518</t>
+  </si>
+  <si>
+    <t>yemi</t>
+  </si>
+  <si>
+    <t>ssg512</t>
+  </si>
+  <si>
+    <t>ssg521</t>
+  </si>
+  <si>
+    <t>ssg515</t>
+  </si>
+  <si>
+    <t>ssg519</t>
+  </si>
+  <si>
+    <t>Eniola</t>
+  </si>
+  <si>
+    <t>Wilfred</t>
+  </si>
+  <si>
+    <t>Bola</t>
+  </si>
+  <si>
+    <t>Anita</t>
+  </si>
+  <si>
+    <t>ssg500</t>
+  </si>
+  <si>
+    <t>ssg511</t>
+  </si>
+  <si>
+    <t>ssg522</t>
+  </si>
+  <si>
+    <t>ssg505</t>
+  </si>
+  <si>
+    <t>Ajibola</t>
+  </si>
+  <si>
+    <t>Fash</t>
+  </si>
+  <si>
+    <t>Adeleye</t>
+  </si>
+  <si>
+    <t>Asaolu</t>
+  </si>
+  <si>
+    <t>sssg 505</t>
+  </si>
+  <si>
+    <t>ssg520</t>
+  </si>
+  <si>
+    <t>ssg523</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>sola</t>
+  </si>
+  <si>
+    <t>harris</t>
+  </si>
+  <si>
+    <t>olumide</t>
+  </si>
+  <si>
+    <t>precious</t>
+  </si>
+  <si>
+    <t>kenny</t>
+  </si>
+  <si>
+    <t>tope</t>
+  </si>
+  <si>
+    <t>wendy</t>
+  </si>
+  <si>
+    <t>jessica</t>
+  </si>
+  <si>
+    <t>Tobi</t>
+  </si>
+  <si>
+    <t>PHS301</t>
+  </si>
+  <si>
+    <t>PHS304</t>
+  </si>
+  <si>
+    <t>PHS302</t>
+  </si>
+  <si>
+    <t>PHS322</t>
+  </si>
+  <si>
+    <t>PHS321</t>
+  </si>
+  <si>
+    <t>PHS305</t>
+  </si>
+  <si>
+    <t>PHS307</t>
+  </si>
+  <si>
+    <t>PHS309</t>
+  </si>
+  <si>
+    <t>PHS3010</t>
+  </si>
+  <si>
+    <t>PHS308</t>
+  </si>
+  <si>
+    <t>Adewale</t>
+  </si>
+  <si>
+    <t>Shittu</t>
+  </si>
+  <si>
+    <t>Dosumu</t>
+  </si>
+  <si>
+    <t>Ogundimu</t>
+  </si>
+  <si>
+    <t>Majidun</t>
+  </si>
+  <si>
+    <t>Olaide</t>
+  </si>
+  <si>
+    <t>EST213</t>
+  </si>
+  <si>
+    <t>EST223</t>
+  </si>
+  <si>
+    <t>EST215</t>
+  </si>
+  <si>
+    <t>EST217</t>
+  </si>
+  <si>
+    <t>EST206</t>
+  </si>
+  <si>
+    <t>EST205</t>
+  </si>
+  <si>
+    <t>Tejuoso</t>
+  </si>
+  <si>
+    <t>PHY401</t>
+  </si>
+  <si>
+    <t>PHY403</t>
+  </si>
+  <si>
+    <t>PHY407</t>
+  </si>
+  <si>
+    <t>PHY421</t>
+  </si>
+  <si>
+    <t>PHY422</t>
+  </si>
+  <si>
+    <t>PHY431</t>
+  </si>
+  <si>
+    <t>Wemimo</t>
+  </si>
+  <si>
+    <t>AGR431</t>
+  </si>
+  <si>
+    <t>MSM432</t>
+  </si>
+  <si>
+    <t>AGR408</t>
+  </si>
+  <si>
+    <t>AGR405</t>
+  </si>
+  <si>
+    <t>MSM411</t>
+  </si>
+  <si>
+    <t>Sopade</t>
+  </si>
+  <si>
+    <t>CSC301</t>
+  </si>
+  <si>
+    <t>CSC302</t>
+  </si>
+  <si>
+    <t>CSC304</t>
+  </si>
+  <si>
+    <t>CSC321</t>
+  </si>
+  <si>
+    <t>MAT311</t>
+  </si>
+  <si>
+    <t>Danladi</t>
+  </si>
+  <si>
+    <t>PHY305</t>
+  </si>
+  <si>
+    <t>Ayomide</t>
+  </si>
+  <si>
+    <t>MST411</t>
+  </si>
+  <si>
+    <t>MST422</t>
+  </si>
+  <si>
+    <t>MST413</t>
+  </si>
+  <si>
+    <t>MST425</t>
+  </si>
+  <si>
+    <t>Chidi</t>
+  </si>
+  <si>
+    <t>CSC522</t>
+  </si>
+  <si>
+    <t>CSC531</t>
+  </si>
+  <si>
+    <t>CSC512</t>
+  </si>
+  <si>
+    <t>PHY206</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>LAW411</t>
+  </si>
+  <si>
+    <t>LAW412</t>
+  </si>
+  <si>
+    <t>CSC307</t>
+  </si>
+  <si>
+    <t>ENG412</t>
+  </si>
+  <si>
+    <t>ENG431</t>
+  </si>
+  <si>
+    <t>LAW425</t>
+  </si>
+  <si>
+    <t>Sadekemi</t>
+  </si>
+  <si>
+    <t>MIC212</t>
+  </si>
+  <si>
+    <t>MIC217</t>
+  </si>
+  <si>
+    <t>MIC231</t>
+  </si>
+  <si>
+    <t>AGR207</t>
+  </si>
+  <si>
+    <t>MAT203</t>
+  </si>
+  <si>
+    <t>BCH205</t>
+  </si>
+  <si>
+    <t>Dogunmu</t>
+  </si>
+  <si>
+    <t>MAT303</t>
+  </si>
+  <si>
+    <t>MIC317</t>
+  </si>
+  <si>
+    <t>MST402</t>
+  </si>
+  <si>
+    <t>MST512</t>
+  </si>
+  <si>
+    <t>MST217</t>
+  </si>
+  <si>
+    <t>Durojaye</t>
+  </si>
+  <si>
+    <t>MST212</t>
+  </si>
+  <si>
+    <t>Soladoye</t>
+  </si>
+  <si>
+    <t>Tejubiyi</t>
+  </si>
+  <si>
+    <t>Merrister</t>
+  </si>
+  <si>
+    <t>Akinpelu</t>
+  </si>
+  <si>
+    <t>Maxwell</t>
+  </si>
+  <si>
+    <t>Makinde</t>
+  </si>
+  <si>
+    <t>Iredele</t>
+  </si>
+  <si>
+    <t>Juliana</t>
+  </si>
+  <si>
+    <t>Oluwaseyi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,7 +601,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -476,11 +904,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -520,6 +959,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -833,11 +1274,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,9 +1321,11 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="3">
+        <v>400</v>
+      </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>4</v>
@@ -901,8 +1344,11 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>38</v>
+      </c>
       <c r="B4" s="2">
-        <v>5</v>
+        <v>400</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
@@ -925,10 +1371,10 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2">
-        <v>6</v>
+        <v>400</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -951,7 +1397,10 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>40</v>
+      </c>
+      <c r="B6" s="2">
+        <v>400</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
@@ -974,10 +1423,10 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2">
-        <v>8</v>
+        <v>400</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>3</v>
@@ -1000,10 +1449,10 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2">
-        <v>9</v>
+        <v>400</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>3</v>
@@ -1023,10 +1472,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2">
-        <v>10</v>
+        <v>400</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
@@ -1049,10 +1498,10 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2">
-        <v>11</v>
+        <v>400</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>3</v>
@@ -1075,10 +1524,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2">
-        <v>12</v>
+        <v>400</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>3</v>
@@ -1097,6 +1546,772 @@
       </c>
       <c r="H11" s="2">
         <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2">
+        <v>500</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="2">
+        <v>500</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="2">
+        <v>500</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="2">
+        <v>500</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="2">
+        <v>500</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="2">
+        <v>500</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="2">
+        <v>501</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="2">
+        <v>502</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" s="2">
+        <v>503</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="2">
+        <v>504</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="2">
+        <v>300</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I22" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="K22" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="L22" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="2">
+        <v>300</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="2">
+        <v>300</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G24" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="2">
+        <v>300</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="2">
+        <v>300</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H26" s="28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" s="2">
+        <v>300</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B28" s="2">
+        <v>300</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="2">
+        <v>300</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="2">
+        <v>300</v>
+      </c>
+      <c r="C30" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="2">
+        <v>300</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B32" s="2">
+        <v>200</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="2">
+        <v>400</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" s="2">
+        <v>400</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="2">
+        <v>300</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="2">
+        <v>300</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B37" s="2">
+        <v>400</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="2">
+        <v>500</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" s="2">
+        <v>400</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B40" s="2">
+        <v>200</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1110,11 +2325,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,11 +2443,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,7 +2458,7 @@
     <col min="8" max="8" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>28</v>
       </c>
@@ -1255,7 +2470,7 @@
       <c r="G1" s="22"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>29</v>
       </c>
@@ -1268,7 +2483,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1294,7 +2509,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1314,7 +2529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1337,7 +2552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -1360,7 +2575,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
@@ -1383,7 +2598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
@@ -1403,7 +2618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -1426,7 +2641,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>2</v>
       </c>
@@ -1449,7 +2664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1472,6 +2687,308 @@
         <v>6</v>
       </c>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="K16" s="28"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="28"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:G1"/>
@@ -1483,11 +3000,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>